<commit_message>
Added color based stuff
</commit_message>
<xml_diff>
--- a/backend/pick-cal.xlsx
+++ b/backend/pick-cal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myCode\Arfaa Appi\time-from-spreadsheet\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6710DE-CFF3-4F35-8C65-1C6BE1B10D47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96B03C2-6794-4F98-9BD4-AB1AE78EF5C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{54A8708B-BCF7-47C5-B517-3AEF63C85F0C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{54A8708B-BCF7-47C5-B517-3AEF63C85F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="2" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -496,6 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,7 +856,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,11 +864,11 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="18.5703125" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
@@ -1017,7 +1018,7 @@
       </c>
       <c r="I5" s="35" t="str">
         <f>TEXT(H5, "hh:mm:ss AM/PM")</f>
-        <v>12:14:50 PM</v>
+        <v>12:14:50 pm</v>
       </c>
       <c r="J5" s="36" t="s">
         <v>21</v>
@@ -1061,6 +1062,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="41" t="str">
+        <f>TEXT(F6, "hh:mm:ss AM/PM")</f>
+        <v>12:10:07 pm</v>
+      </c>
       <c r="J7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1164,7 @@
       </c>
       <c r="H13" s="12">
         <f ca="1">NOW()</f>
-        <v>45778.609907638885</v>
+        <v>45831.865648148145</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1172,11 +1177,11 @@
       </c>
       <c r="H14" s="13">
         <f ca="1">H13+(H11*H12)</f>
-        <v>45778.697604710957</v>
+        <v>45831.953345220216</v>
       </c>
       <c r="I14" s="34" t="str">
         <f ca="1">TEXT(H14, "hh:mm:ss AM/PM")</f>
-        <v>04:44:33 PM</v>
+        <v>10:52:49 pm</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added railway.json file to push backend to railway
</commit_message>
<xml_diff>
--- a/backend/pick-cal.xlsx
+++ b/backend/pick-cal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myCode\Arfaa Appi\time-from-spreadsheet\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96B03C2-6794-4F98-9BD4-AB1AE78EF5C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5A4C58-375F-45C8-880F-F4A834081AC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{54A8708B-BCF7-47C5-B517-3AEF63C85F0C}"/>
   </bookViews>
@@ -481,6 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,7 +497,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,7 +856,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,26 +878,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="36" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="J1" s="36" t="s">
+      <c r="H1" s="38"/>
+      <c r="J1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="37"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1020,10 +1020,10 @@
         <f>TEXT(H5, "hh:mm:ss AM/PM")</f>
         <v>12:14:50 pm</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
@@ -1062,7 +1062,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="41" t="str">
+      <c r="F7" s="36" t="str">
         <f>TEXT(F6, "hh:mm:ss AM/PM")</f>
         <v>12:10:07 pm</v>
       </c>
@@ -1079,10 +1079,10 @@
       <c r="D8" s="24"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="40"/>
+      <c r="H8" s="41"/>
       <c r="J8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="H13" s="12">
         <f ca="1">NOW()</f>
-        <v>45831.865648148145</v>
+        <v>45834.921005439814</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1177,11 +1177,11 @@
       </c>
       <c r="H14" s="13">
         <f ca="1">H13+(H11*H12)</f>
-        <v>45831.953345220216</v>
+        <v>45835.008702511885</v>
       </c>
       <c r="I14" s="34" t="str">
         <f ca="1">TEXT(H14, "hh:mm:ss AM/PM")</f>
-        <v>10:52:49 pm</v>
+        <v>12:12:32 am</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1199,10 +1199,10 @@
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="37"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="24"/>

</xml_diff>